<commit_message>
structure revamp for future tools and internationalization
</commit_message>
<xml_diff>
--- a/careercrashcourse.com/input.xlsx
+++ b/careercrashcourse.com/input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>url</t>
   </si>
@@ -34,46 +34,49 @@
     <t>updated</t>
   </si>
   <si>
+    <t>saas product design principle</t>
+  </si>
+  <si>
+    <t>intelligent b-side product analysis and design ideas</t>
+  </si>
+  <si>
+    <t>how to design a corporate system ui</t>
+  </si>
+  <si>
+    <t>how to design a 2b data table</t>
+  </si>
+  <si>
+    <t>how to break down complex process</t>
+  </si>
+  <si>
+    <t>business requirement management for corporate systems</t>
+  </si>
+  <si>
+    <t>5 steps to a great sharing function design</t>
+  </si>
+  <si>
+    <t>saas-product-design-principle</t>
+  </si>
+  <si>
+    <t>intelligent-b-side-product-analysis-and-design-ideas</t>
+  </si>
+  <si>
+    <t>how-to-design-a-corporate-system-ui</t>
+  </si>
+  <si>
+    <t>how-to-design-a-2b-data-table</t>
+  </si>
+  <si>
+    <t>how-to-break-down-complex-process</t>
+  </si>
+  <si>
+    <t>business-requirement-management-for-corporate-systems</t>
+  </si>
+  <si>
+    <t>steps-to-a-great-sharing-function-design</t>
+  </si>
+  <si>
     <t>Saas Product Design Principle</t>
-  </si>
-  <si>
-    <t>Intelligent B-side product analysis and design ideas</t>
-  </si>
-  <si>
-    <t>How to design a corporate system UI</t>
-  </si>
-  <si>
-    <t>How to design a 2b data table</t>
-  </si>
-  <si>
-    <t>How to break down complex process</t>
-  </si>
-  <si>
-    <t>Business requirement management for corporate systems</t>
-  </si>
-  <si>
-    <t>5 steps to a great sharing function design</t>
-  </si>
-  <si>
-    <t>saas-product-design-principle</t>
-  </si>
-  <si>
-    <t>intelligent-b-side-product-analysis-and-design-ideas</t>
-  </si>
-  <si>
-    <t>how-to-design-a-corporate-system-ui</t>
-  </si>
-  <si>
-    <t>how-to-design-a-2b-data-table</t>
-  </si>
-  <si>
-    <t>how-to-break-down-complex-process</t>
-  </si>
-  <si>
-    <t>business-requirement-management-for-corporate-systems</t>
-  </si>
-  <si>
-    <t>steps-to-a-great-sharing-function-design</t>
   </si>
   <si>
     <t>Intelligent B-Side Product Analysis And Design Ideas</t>
@@ -490,7 +493,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2">
         <v>44962.8495143871</v>
@@ -510,7 +513,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2">
         <v>44962.84912997793</v>
@@ -530,7 +533,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2">
         <v>44962.84897406979</v>
@@ -550,7 +553,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2">
         <v>44962.84882952934</v>
@@ -570,7 +573,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2">
         <v>44962.84868081223</v>
@@ -590,7 +593,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2">
         <v>44962.8485411623</v>
@@ -610,7 +613,7 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2">
         <v>44962.8483842971</v>

</xml_diff>